<commit_message>
Update mpIF inventory and fix bug with H&E samples from "Other" sites
</commit_message>
<xml_diff>
--- a/tables/patient_metadata.xlsx
+++ b/tables/patient_metadata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">SPECTRUM-OV-002</t>
   </si>
   <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
     <t xml:space="preserve">Primary</t>
   </si>
   <si>
@@ -38,6 +41,9 @@
     <t xml:space="preserve">SPECTRUM-OV-003</t>
   </si>
   <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
     <t xml:space="preserve">NACT/IDS</t>
   </si>
   <si>
@@ -47,33 +53,57 @@
     <t xml:space="preserve">SPECTRUM-OV-004</t>
   </si>
   <si>
+    <t xml:space="preserve">73</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-006</t>
   </si>
   <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-007</t>
   </si>
   <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-008</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-009</t>
   </si>
   <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-011</t>
   </si>
   <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-014</t>
   </si>
   <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-015</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-016</t>
   </si>
   <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-018</t>
   </si>
   <si>
+    <t xml:space="preserve">62</t>
+  </si>
+  <si>
     <t xml:space="preserve">IIIB</t>
   </si>
   <si>
@@ -83,21 +113,36 @@
     <t xml:space="preserve">SPECTRUM-OV-022</t>
   </si>
   <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-024</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-025</t>
   </si>
   <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-026</t>
   </si>
   <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-028</t>
   </si>
   <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-029</t>
   </si>
   <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-030</t>
   </si>
   <si>
@@ -107,18 +152,30 @@
     <t xml:space="preserve">SPECTRUM-OV-032</t>
   </si>
   <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-033</t>
   </si>
   <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-034</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-036</t>
   </si>
   <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-037</t>
   </si>
   <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-038</t>
   </si>
   <si>
@@ -137,9 +194,15 @@
     <t xml:space="preserve">SPECTRUM-OV-045</t>
   </si>
   <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-046</t>
   </si>
   <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-048</t>
   </si>
   <si>
@@ -152,9 +215,15 @@
     <t xml:space="preserve">SPECTRUM-OV-051</t>
   </si>
   <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-052</t>
   </si>
   <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-053</t>
   </si>
   <si>
@@ -167,6 +236,9 @@
     <t xml:space="preserve">SPECTRUM-OV-056</t>
   </si>
   <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-059</t>
   </si>
   <si>
@@ -179,18 +251,30 @@
     <t xml:space="preserve">SPECTRUM-OV-064</t>
   </si>
   <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-065</t>
   </si>
   <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-066</t>
   </si>
   <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-067</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-068</t>
   </si>
   <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-070</t>
   </si>
   <si>
@@ -203,9 +287,15 @@
     <t xml:space="preserve">SPECTRUM-OV-073</t>
   </si>
   <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-075</t>
   </si>
   <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-077</t>
   </si>
   <si>
@@ -221,6 +311,9 @@
     <t xml:space="preserve">SPECTRUM-OV-083</t>
   </si>
   <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-090</t>
   </si>
   <si>
@@ -276,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-118</t>
@@ -628,1092 +724,1092 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>68</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>63</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="n">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="n">
-        <v>66</v>
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="n">
-        <v>45</v>
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="n">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="n">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="n">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="n">
-        <v>82</v>
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="n">
-        <v>49</v>
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="n">
-        <v>59</v>
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="n">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="n">
-        <v>49</v>
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="n">
-        <v>57</v>
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="n">
-        <v>82</v>
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="n">
-        <v>74</v>
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="n">
-        <v>55</v>
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="n">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="n">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="n">
-        <v>69</v>
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="n">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="n">
-        <v>77</v>
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" t="n">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" t="n">
-        <v>68</v>
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="n">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="n">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" t="n">
         <v>54</v>
       </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="n">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="n">
-        <v>77</v>
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="n">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="n">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" t="n">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" t="n">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" t="n">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" t="n">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" t="n">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
         <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="n">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" t="n">
-        <v>44</v>
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" t="n">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="n">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" t="n">
-        <v>53</v>
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" t="n">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" t="n">
-        <v>68</v>
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" t="n">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" t="n">
-        <v>75</v>
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" t="n">
-        <v>52</v>
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" t="n">
-        <v>69</v>
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" t="n">
-        <v>69</v>
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" t="n">
-        <v>69</v>
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" t="n">
-        <v>68</v>
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" t="n">
-        <v>61</v>
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" t="n">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" t="n">
-        <v>40</v>
+        <v>92</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" t="n">
-        <v>58</v>
+        <v>94</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" t="n">
-        <v>56</v>
+        <v>95</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" t="n">
-        <v>65</v>
+        <v>96</v>
+      </c>
+      <c r="B57" t="s">
+        <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" t="n">
-        <v>67</v>
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" t="n">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" t="n">
-        <v>69</v>
+        <v>100</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" t="n">
-        <v>68</v>
+        <v>101</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" t="n">
-        <v>49</v>
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B63" t="n">
-        <v>75</v>
+        <v>103</v>
+      </c>
+      <c r="B63" t="s">
+        <v>81</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" t="n">
-        <v>59</v>
+        <v>104</v>
+      </c>
+      <c r="B64" t="s">
+        <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" t="n">
-        <v>69</v>
+        <v>105</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" t="n">
-        <v>70</v>
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" t="n">
-        <v>42</v>
+        <v>107</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" t="n">
+        <v>108</v>
+      </c>
+      <c r="B68" t="s">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>78</v>
-      </c>
-      <c r="B69" t="n">
-        <v>66</v>
+        <v>109</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" t="n">
-        <v>55</v>
+        <v>110</v>
+      </c>
+      <c r="B70" t="s">
+        <v>60</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" t="n">
-        <v>55</v>
+        <v>111</v>
+      </c>
+      <c r="B71" t="s">
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" t="n">
-        <v>59</v>
+        <v>112</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>82</v>
-      </c>
-      <c r="B73" t="n">
-        <v>56</v>
+        <v>113</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" t="n">
-        <v>63</v>
+        <v>114</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>84</v>
-      </c>
-      <c r="B75" t="n">
-        <v>68</v>
+        <v>115</v>
+      </c>
+      <c r="B75" t="s">
+        <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>85</v>
-      </c>
-      <c r="B76" t="n">
-        <v>53</v>
+        <v>116</v>
+      </c>
+      <c r="B76" t="s">
+        <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" t="n">
-        <v>54</v>
+        <v>117</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
       </c>
       <c r="C77" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" t="n">
-        <v>46</v>
+        <v>118</v>
+      </c>
+      <c r="B78" t="s">
+        <v>119</v>
       </c>
       <c r="C78" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" t="n">
-        <v>58</v>
+        <v>120</v>
+      </c>
+      <c r="B79" t="s">
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to sample metadata tables
</commit_message>
<xml_diff>
--- a/tables/patient_metadata.xlsx
+++ b/tables/patient_metadata.xlsx
@@ -206,6 +206,9 @@
     <t xml:space="preserve">SPECTRUM-OV-048</t>
   </si>
   <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-049</t>
   </si>
   <si>
@@ -252,9 +255,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-066</t>
@@ -1170,7 +1170,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
         <v>17</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -1260,15 +1260,15 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
         <v>39</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -1335,10 +1335,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -1408,7 +1408,7 @@
         <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -1422,7 +1422,7 @@
         <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -1576,7 +1576,7 @@
         <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
@@ -1596,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65">
@@ -1646,7 +1646,7 @@
         <v>106</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
@@ -1708,7 +1708,7 @@
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73">
@@ -1736,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75">

</xml_diff>

<commit_message>
Add tumor_megasite to database and tables
</commit_message>
<xml_diff>
--- a/tables/patient_metadata.xlsx
+++ b/tables/patient_metadata.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
   <si>
+    <t xml:space="preserve">patient_isabl_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">patient_age</t>
   </si>
   <si>
@@ -29,7 +32,7 @@
     <t xml:space="preserve">SPECTRUM-OV-002</t>
   </si>
   <si>
-    <t xml:space="preserve">70</t>
+    <t xml:space="preserve">SHAH_H000004</t>
   </si>
   <si>
     <t xml:space="preserve">Primary</t>
@@ -41,7 +44,7 @@
     <t xml:space="preserve">SPECTRUM-OV-003</t>
   </si>
   <si>
-    <t xml:space="preserve">64</t>
+    <t xml:space="preserve">SHAH_H000005</t>
   </si>
   <si>
     <t xml:space="preserve">NACT/IDS</t>
@@ -53,34 +56,37 @@
     <t xml:space="preserve">SPECTRUM-OV-004</t>
   </si>
   <si>
-    <t xml:space="preserve">74</t>
+    <t xml:space="preserve">SHAH_H000029</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-007</t>
   </si>
   <si>
-    <t xml:space="preserve">46</t>
+    <t xml:space="preserve">SHAH_H000006</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-008</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000011</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-009</t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
+    <t xml:space="preserve">SHAH_H000013</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-014</t>
   </si>
   <si>
-    <t xml:space="preserve">84</t>
+    <t xml:space="preserve">SHAH_H000009</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-022</t>
   </si>
   <si>
-    <t xml:space="preserve">58</t>
+    <t xml:space="preserve">SHAH_H000019</t>
   </si>
   <si>
     <t xml:space="preserve">IIIB</t>
@@ -89,163 +95,208 @@
     <t xml:space="preserve">SPECTRUM-OV-024</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000020</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-025</t>
   </si>
   <si>
-    <t xml:space="preserve">75</t>
+    <t xml:space="preserve">SHAH_H000021</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-026</t>
   </si>
   <si>
-    <t xml:space="preserve">56</t>
+    <t xml:space="preserve">SHAH_H000022</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-031</t>
   </si>
   <si>
-    <t xml:space="preserve">55</t>
+    <t xml:space="preserve">SHAH_H000023</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-036</t>
   </si>
   <si>
-    <t xml:space="preserve">77</t>
+    <t xml:space="preserve">SHAH_H000039</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-037</t>
   </si>
   <si>
-    <t xml:space="preserve">45</t>
+    <t xml:space="preserve">SHAH_H000024</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-041</t>
   </si>
   <si>
-    <t xml:space="preserve">63</t>
+    <t xml:space="preserve">SHAH_H000025</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-042</t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
+    <t xml:space="preserve">SHAH_H000026</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-045</t>
   </si>
   <si>
-    <t xml:space="preserve">57</t>
+    <t xml:space="preserve">SHAH_H000031</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-049</t>
   </si>
   <si>
-    <t xml:space="preserve">67</t>
+    <t xml:space="preserve">SHAH_H000036</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-050</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000033</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-051</t>
   </si>
   <si>
-    <t xml:space="preserve">68</t>
+    <t xml:space="preserve">SHAH_H000034</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-052</t>
   </si>
   <si>
-    <t xml:space="preserve">61</t>
+    <t xml:space="preserve">SHAH_H000035</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-053</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000037</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-054</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000038</t>
+  </si>
+  <si>
     <t xml:space="preserve">IVA</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-065</t>
   </si>
   <si>
-    <t xml:space="preserve">76</t>
+    <t xml:space="preserve">SHAH_H000041</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-067</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000149</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-068</t>
   </si>
   <si>
-    <t xml:space="preserve">71</t>
+    <t xml:space="preserve">SHAH_H000180</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-070</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000181</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-071</t>
   </si>
   <si>
-    <t xml:space="preserve">69</t>
+    <t xml:space="preserve">SHAH_H000182</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-075</t>
   </si>
   <si>
-    <t xml:space="preserve">41</t>
+    <t xml:space="preserve">SHAH_H000213</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-077</t>
   </si>
   <si>
-    <t xml:space="preserve">60</t>
+    <t xml:space="preserve">SHAH_H000214</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-080</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000338</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-081</t>
   </si>
   <si>
-    <t xml:space="preserve">66</t>
+    <t xml:space="preserve">SHAH_H000340</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-082</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000339</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-083</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000342</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-090</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000408</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-105</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000705</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-107</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000708</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-110</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000706</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-112</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H000707</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-115</t>
   </si>
   <si>
-    <t xml:space="preserve">54</t>
+    <t xml:space="preserve">SHAH_H001749</t>
   </si>
   <si>
     <t xml:space="preserve">SPECTRUM-OV-116</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAH_H001750</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-118</t>
   </si>
   <si>
-    <t xml:space="preserve">59</t>
+    <t xml:space="preserve">SHAH_H001753</t>
   </si>
 </sst>
 </file>
@@ -590,593 +641,722 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="n">
+        <v>70</v>
+      </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
         <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="n">
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="C6" t="n">
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C8" t="n">
+        <v>84</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="C9" t="n">
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="C10" t="n">
+        <v>84</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="C11" t="n">
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="C12" t="n">
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="C13" t="n">
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="C14" t="n">
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
+        <v>37</v>
+      </c>
+      <c r="C15" t="n">
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="C16" t="n">
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="C17" t="n">
+        <v>78</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
+        <v>43</v>
+      </c>
+      <c r="C18" t="n">
+        <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
+        <v>45</v>
+      </c>
+      <c r="C19" t="n">
+        <v>68</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="C20" t="n">
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="C21" t="n">
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
+        <v>51</v>
+      </c>
+      <c r="C22" t="n">
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
+        <v>53</v>
+      </c>
+      <c r="C23" t="n">
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+      <c r="C24" t="n">
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="C25" t="n">
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="C26" t="n">
+        <v>70</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="C27" t="n">
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="C28" t="n">
+        <v>70</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
+        <v>66</v>
+      </c>
+      <c r="C29" t="n">
+        <v>70</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
+        <v>68</v>
+      </c>
+      <c r="C30" t="n">
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
+        <v>70</v>
+      </c>
+      <c r="C31" t="n">
+        <v>60</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
+        <v>72</v>
+      </c>
+      <c r="C32" t="n">
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
+        <v>74</v>
+      </c>
+      <c r="C33" t="n">
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
+        <v>76</v>
+      </c>
+      <c r="C34" t="n">
+        <v>69</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="C35" t="n">
+        <v>60</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
+        <v>80</v>
+      </c>
+      <c r="C36" t="n">
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="C37" t="n">
+        <v>57</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
+        <v>84</v>
+      </c>
+      <c r="C38" t="n">
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
+        <v>86</v>
+      </c>
+      <c r="C39" t="n">
+        <v>58</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
+        <v>88</v>
+      </c>
+      <c r="C40" t="n">
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
+        <v>90</v>
+      </c>
+      <c r="C41" t="n">
+        <v>55</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
+        <v>92</v>
+      </c>
+      <c r="C42" t="n">
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="C43" t="n">
+        <v>59</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add patient DMP ID to tables and fix minor issues with tumor subsite of two H&E/mpIF samples
</commit_message>
<xml_diff>
--- a/tables/patient_metadata.xlsx
+++ b/tables/patient_metadata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -20,6 +20,9 @@
     <t xml:space="preserve">patient_isabl_id</t>
   </si>
   <si>
+    <t xml:space="preserve">patient_dmp_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">patient_age</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
     <t xml:space="preserve">SHAH_H000004</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0039615</t>
+  </si>
+  <si>
     <t xml:space="preserve">Primary</t>
   </si>
   <si>
@@ -47,6 +53,9 @@
     <t xml:space="preserve">SHAH_H000005</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0039726</t>
+  </si>
+  <si>
     <t xml:space="preserve">NACT/IDS</t>
   </si>
   <si>
@@ -59,36 +68,54 @@
     <t xml:space="preserve">SHAH_H000029</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0039734</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-007</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000006</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0040980</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-008</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000011</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0041572</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-009</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000013</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0042164</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-014</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000009</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0042548</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-022</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000019</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0043571</t>
+  </si>
+  <si>
     <t xml:space="preserve">IIIB</t>
   </si>
   <si>
@@ -98,90 +125,135 @@
     <t xml:space="preserve">SHAH_H000020</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0044784</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-025</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000021</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0044084</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-026</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000022</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0043587</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-031</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000023</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0045494</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-036</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000039</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0045589</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-037</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000024</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0046401</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-041</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000025</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0047883</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-042</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000026</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0046857</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-045</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000031</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0047947</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-049</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000036</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0048524</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-050</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000033</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0051015</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-051</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000034</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0048525</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-052</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000035</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0048670</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-053</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000037</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0048695</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-054</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000038</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0048554</t>
+  </si>
+  <si>
     <t xml:space="preserve">IVA</t>
   </si>
   <si>
@@ -191,112 +263,169 @@
     <t xml:space="preserve">SHAH_H000041</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0051130</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-067</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000149</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0052274</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-068</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000180</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0052385</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-070</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000181</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0052359</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-071</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000182</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0052808</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-075</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000213</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0054073</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-077</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000214</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0054406</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-080</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000338</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0055809</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-081</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000340</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0056102</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-082</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000339</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0055908</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-083</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000342</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0056224</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-090</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000408</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0056958</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-105</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000705</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0059884</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-107</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000708</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0060366</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-110</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000706</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0059753</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-112</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H000707</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0060511</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-115</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H001749</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0060627</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-116</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H001750</t>
   </si>
   <si>
+    <t xml:space="preserve">P-0060931</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPECTRUM-OV-118</t>
   </si>
   <si>
     <t xml:space="preserve">SHAH_H001753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-0061784</t>
   </si>
 </sst>
 </file>
@@ -644,719 +773,848 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="n">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="n">
         <v>64</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="n">
         <v>74</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="n">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="n">
         <v>65</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="n">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="n">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="n">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="n">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="n">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="n">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="n">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="n">
         <v>84</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="n">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="n">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="n">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="n">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="n">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="n">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="n">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="n">
         <v>77</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="n">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="n">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="n">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="n">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="n">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="n">
         <v>78</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="n">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="n">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="n">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="n">
         <v>68</v>
       </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="n">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="n">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" t="n">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="n">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="n">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="n">
         <v>61</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" t="n">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="n">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" t="n">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="n">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="n">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="n">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" t="n">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="n">
         <v>70</v>
       </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="n">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="n">
         <v>71</v>
       </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="n">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="n">
         <v>70</v>
       </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" t="n">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="n">
         <v>70</v>
       </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" t="n">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="n">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="n">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="n">
         <v>60</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="n">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="n">
         <v>57</v>
       </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" t="n">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="n">
         <v>66</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="n">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="n">
         <v>69</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" t="n">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="n">
         <v>60</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" t="n">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="n">
         <v>70</v>
       </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" t="n">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" t="n">
         <v>57</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" t="n">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" t="n">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" t="n">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" t="n">
         <v>58</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" t="n">
+        <v>127</v>
+      </c>
+      <c r="C40" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" t="n">
         <v>69</v>
       </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" t="n">
+        <v>130</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="n">
         <v>55</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" t="n">
+        <v>133</v>
+      </c>
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" t="n">
         <v>56</v>
       </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" t="n">
+        <v>136</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="n">
         <v>59</v>
       </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>